<commit_message>
qq maj sur artefcat 1 et le plan de travail (typos)
</commit_message>
<xml_diff>
--- a/Document/PlanDeTravail.xlsx
+++ b/Document/PlanDeTravail.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Feuil2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Feuil3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
+    <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -33,12 +32,12 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">(échéance : 16 Octobre)</t>
+      <t>(échéance : 16 Octobre)</t>
     </r>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Itération 2</t>
+      <t>Itération 2</t>
     </r>
     <r>
       <rPr>
@@ -53,7 +52,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Itération 3</t>
+      <t>Itération 3</t>
     </r>
     <r>
       <rPr>
@@ -85,9 +84,6 @@
     <t>10 jours</t>
   </si>
   <si>
-    <t>Résumé l'activité de l'usine et afficher les information</t>
-  </si>
-  <si>
     <t>Vérifier la cohérence du plan</t>
   </si>
   <si>
@@ -134,16 +130,16 @@
   </si>
   <si>
     <t>2 jour</t>
+  </si>
+  <si>
+    <t>Résumer l'activité de l'usine et afficher les information</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-  </numFmts>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -152,22 +148,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
@@ -215,126 +196,77 @@
     </fill>
   </fills>
   <borders count="4">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="dotted"/>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
-      <top style="dotted"/>
-      <bottom style="dotted"/>
+      <top style="dotted">
+        <color auto="1"/>
+      </top>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
-      <top style="dotted"/>
+      <top style="dotted">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="14">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -393,65 +325,362 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
   <dimension ref="A3:H17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="4.10204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.6683673469388"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.55612244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.6683673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.55612244897959"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="24.6683673469388"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.89285714285714"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="4.10204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="26.5561224489796"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.66836734693878"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.89285714285714"/>
+    <col min="1" max="1" width="4.140625"/>
+    <col min="2" max="2" width="24.7109375"/>
+    <col min="3" max="3" width="8.5703125"/>
+    <col min="4" max="4" width="24.7109375"/>
+    <col min="5" max="5" width="8.5703125"/>
+    <col min="6" max="6" width="25.85546875" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875"/>
+    <col min="8" max="8" width="4.140625"/>
+    <col min="9" max="9" width="26.5703125"/>
+    <col min="10" max="10" width="7.7109375"/>
+    <col min="11" max="1025" width="8.85546875"/>
   </cols>
   <sheetData>
-    <row r="3" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="2" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2" t="s">
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2" t="s">
+      <c r="E6" s="1"/>
+      <c r="F6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
@@ -471,7 +700,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>6</v>
       </c>
@@ -491,7 +720,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>8</v>
       </c>
@@ -499,89 +728,89 @@
         <v>9</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="9" t="s">
+    </row>
+    <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="8" t="s">
+      <c r="C10" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="D10" s="8" t="s">
         <v>14</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>15</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>7</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="D11" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="E11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" s="10" t="s">
+      <c r="G11" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G11" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="8" t="s">
-        <v>21</v>
-      </c>
       <c r="C12" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="9"/>
     </row>
-    <row r="13" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="9"/>
       <c r="F13" s="10"/>
       <c r="G13" s="9"/>
     </row>
-    <row r="14" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>7</v>
@@ -591,9 +820,9 @@
       <c r="F14" s="10"/>
       <c r="G14" s="9"/>
     </row>
-    <row r="15" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>7</v>
@@ -603,9 +832,9 @@
       <c r="F15" s="10"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>7</v>
@@ -615,12 +844,12 @@
       <c r="F16" s="10"/>
       <c r="G16" s="9"/>
     </row>
-    <row r="17" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D17" s="13"/>
       <c r="E17" s="12"/>
@@ -634,66 +863,45 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="F6:G6"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.89285714285714"/>
+    <col min="1" max="1025" width="8.85546875"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.89285714285714"/>
+    <col min="1" max="1025" width="8.85546875"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>